<commit_message>
filtered df_pivot_filtered_numbers by the specific metric, modified polynomial.ipynb to adjust for missing values
</commit_message>
<xml_diff>
--- a/data/DATA_PKD_SPECIFIC.xlsx
+++ b/data/DATA_PKD_SPECIFIC.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wojte\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Documents/competitions/hackatons/hacknation_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC141743-7CF6-4AC6-8708-1158587622E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C2F80D-31BA-5340-A339-E3D6F26277F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,9 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
-    <t>Export_mln_PLN</t>
-  </si>
-  <si>
     <t>przewieziona masa towarów mln ton</t>
   </si>
   <si>
@@ -192,6 +190,9 @@
   </si>
   <si>
     <t>https://data.ecb.europa.eu/data/datasets/ICP/ICP.A.PL.N.071100.4.INW</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -548,23 +549,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED60E7D-B85A-4F1E-AE0A-0124CD153205}">
-  <dimension ref="A1:AG174"/>
+  <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="1"/>
-    <col min="7" max="7" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="20.5" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.6640625" style="1"/>
+    <col min="6" max="6" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +581,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
@@ -589,10 +592,10 @@
       <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
       <c r="L1" t="s">
@@ -658,1534 +661,1405 @@
       <c r="AF1" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2012</v>
       </c>
+      <c r="B2" s="1">
+        <v>231.29938883599999</v>
+      </c>
       <c r="C2" s="1">
-        <v>231.29938883599999</v>
+        <v>4.25</v>
       </c>
       <c r="D2" s="1">
-        <v>4.25</v>
+        <v>1712.13</v>
       </c>
       <c r="E2" s="1">
-        <v>1712.13</v>
-      </c>
-      <c r="F2" s="1">
         <v>595</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2">
         <v>103</v>
       </c>
-      <c r="J2" s="1">
+      <c r="I2" s="1">
         <v>2294.5</v>
       </c>
-      <c r="K2" s="5">
+      <c r="J2" s="5">
         <v>7536</v>
       </c>
+      <c r="K2">
+        <v>201.36</v>
+      </c>
       <c r="L2">
-        <v>201.36</v>
+        <v>3.37</v>
       </c>
       <c r="M2">
-        <v>3.37</v>
+        <v>92.5</v>
       </c>
       <c r="N2">
-        <v>92.5</v>
+        <v>3.6</v>
       </c>
       <c r="O2">
-        <v>3.6</v>
+        <v>3.2518400000000001</v>
       </c>
       <c r="P2">
-        <v>3.2518400000000001</v>
+        <v>4.1849999999999996</v>
       </c>
       <c r="Q2">
-        <v>4.1849999999999996</v>
+        <v>267502217</v>
       </c>
       <c r="R2">
-        <v>267502217</v>
+        <v>757239</v>
       </c>
       <c r="S2">
-        <v>757239</v>
+        <v>7757588</v>
       </c>
       <c r="T2">
-        <v>7757588</v>
+        <v>18744412</v>
       </c>
       <c r="U2">
-        <v>18744412</v>
+        <v>5.73</v>
       </c>
       <c r="V2">
-        <v>5.73</v>
-      </c>
-      <c r="W2">
         <v>18.350000000000001</v>
       </c>
+      <c r="W2" s="6">
+        <v>89.34</v>
+      </c>
       <c r="X2" s="6">
-        <v>89.34</v>
+        <v>33.979999999999997</v>
       </c>
       <c r="Y2" s="6">
-        <v>33.979999999999997</v>
+        <v>13.72</v>
       </c>
       <c r="Z2" s="6">
-        <v>13.72</v>
+        <v>671.61</v>
       </c>
       <c r="AA2" s="6">
-        <v>671.61</v>
+        <v>1169.21</v>
       </c>
       <c r="AB2" s="6">
-        <v>1169.21</v>
+        <v>6.4</v>
       </c>
       <c r="AC2" s="6">
-        <v>6.4</v>
+        <v>1.2</v>
       </c>
       <c r="AD2" s="6">
-        <v>1.2</v>
+        <v>0.66</v>
       </c>
       <c r="AE2" s="6">
-        <v>0.66</v>
+        <v>19.41</v>
       </c>
       <c r="AF2" s="6">
-        <v>19.41</v>
-      </c>
-      <c r="AG2" s="6">
         <v>353.36</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2013</v>
       </c>
+      <c r="B3" s="1">
+        <v>233.16539897399997</v>
+      </c>
       <c r="C3" s="1">
-        <v>233.16539897399997</v>
+        <v>2.5</v>
       </c>
       <c r="D3" s="1">
-        <v>2.5</v>
+        <v>1765.86</v>
       </c>
       <c r="E3" s="1">
-        <v>1765.86</v>
-      </c>
-      <c r="F3" s="1">
         <v>585</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
         <v>103.5</v>
       </c>
-      <c r="J3" s="3">
+      <c r="I3" s="3">
         <v>2091</v>
       </c>
-      <c r="K3" s="5">
+      <c r="J3" s="5">
         <v>7192</v>
       </c>
+      <c r="K3">
+        <v>181.55</v>
+      </c>
       <c r="L3">
-        <v>181.55</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="M3">
-        <v>4.0999999999999996</v>
+        <v>81.69</v>
       </c>
       <c r="N3">
-        <v>81.69</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>3.1602800000000002</v>
       </c>
       <c r="P3">
-        <v>3.1602800000000002</v>
+        <v>4.1974999999999998</v>
       </c>
       <c r="Q3">
-        <v>4.1974999999999998</v>
+        <v>272931265</v>
       </c>
       <c r="R3">
-        <v>272931265</v>
+        <v>827080</v>
       </c>
       <c r="S3">
-        <v>827080</v>
+        <v>7453835</v>
       </c>
       <c r="T3">
-        <v>7453835</v>
+        <v>19389446</v>
       </c>
       <c r="U3">
-        <v>19389446</v>
+        <v>5.51</v>
       </c>
       <c r="V3">
-        <v>5.51</v>
-      </c>
-      <c r="W3">
         <v>19.68</v>
       </c>
+      <c r="W3" s="6">
+        <v>79.67</v>
+      </c>
       <c r="X3" s="6">
-        <v>79.67</v>
+        <v>48.85</v>
       </c>
       <c r="Y3" s="6">
-        <v>48.85</v>
+        <v>14.87</v>
       </c>
       <c r="Z3" s="6">
-        <v>14.87</v>
+        <v>671.95</v>
       </c>
       <c r="AA3" s="6">
-        <v>671.95</v>
+        <v>1136.03</v>
       </c>
       <c r="AB3" s="6">
-        <v>1136.03</v>
+        <v>6.2</v>
       </c>
       <c r="AC3" s="6">
-        <v>6.2</v>
+        <v>1.36</v>
       </c>
       <c r="AD3" s="6">
-        <v>1.36</v>
+        <v>0.67</v>
       </c>
       <c r="AE3" s="6">
-        <v>0.67</v>
+        <v>20.51</v>
       </c>
       <c r="AF3" s="6">
-        <v>20.51</v>
-      </c>
-      <c r="AG3" s="6">
         <v>344.98</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2014</v>
       </c>
+      <c r="B4" s="1">
+        <v>228.866018685</v>
+      </c>
       <c r="C4" s="1">
-        <v>228.866018685</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>1855.92</v>
       </c>
       <c r="E4" s="1">
-        <v>1855.92</v>
-      </c>
-      <c r="F4" s="1">
         <v>674</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2">
         <v>100.7</v>
       </c>
-      <c r="J4" s="3">
+      <c r="I4" s="3">
         <v>1706</v>
       </c>
-      <c r="K4" s="5">
+      <c r="J4" s="5">
         <v>7265</v>
       </c>
+      <c r="K4">
+        <v>163.58000000000001</v>
+      </c>
       <c r="L4">
-        <v>163.58000000000001</v>
+        <v>2.92</v>
       </c>
       <c r="M4">
-        <v>2.92</v>
+        <v>75.38</v>
       </c>
       <c r="N4">
-        <v>75.38</v>
+        <v>0.1</v>
       </c>
       <c r="O4">
-        <v>0.1</v>
+        <v>3.1542699999999999</v>
       </c>
       <c r="P4">
-        <v>3.1542699999999999</v>
+        <v>4.1852</v>
       </c>
       <c r="Q4">
-        <v>4.1852</v>
+        <v>286955865</v>
       </c>
       <c r="R4">
-        <v>286955865</v>
+        <v>760056</v>
       </c>
       <c r="S4">
-        <v>760056</v>
+        <v>6894371</v>
       </c>
       <c r="T4">
-        <v>6894371</v>
+        <v>20003863</v>
       </c>
       <c r="U4">
-        <v>20003863</v>
+        <v>5.3</v>
       </c>
       <c r="V4">
-        <v>5.3</v>
-      </c>
-      <c r="W4">
         <v>17.71</v>
       </c>
+      <c r="W4" s="6">
+        <v>68.36</v>
+      </c>
       <c r="X4" s="6">
-        <v>68.36</v>
+        <v>38.79</v>
       </c>
       <c r="Y4" s="6">
-        <v>38.79</v>
+        <v>12.59</v>
       </c>
       <c r="Z4" s="6">
-        <v>12.59</v>
+        <v>722.93</v>
       </c>
       <c r="AA4" s="6">
-        <v>722.93</v>
+        <v>1292.07</v>
       </c>
       <c r="AB4" s="6">
-        <v>1292.07</v>
+        <v>5.96</v>
       </c>
       <c r="AC4" s="6">
-        <v>5.96</v>
+        <v>1.37</v>
       </c>
       <c r="AD4" s="6">
-        <v>1.37</v>
+        <v>0.64</v>
       </c>
       <c r="AE4" s="6">
-        <v>0.64</v>
+        <v>21.15</v>
       </c>
       <c r="AF4" s="6">
-        <v>21.15</v>
-      </c>
-      <c r="AG4" s="6">
         <v>347.39</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2015</v>
       </c>
+      <c r="B5" s="1">
+        <v>224.77729533899998</v>
+      </c>
       <c r="C5" s="1">
-        <v>224.77729533899998</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="1">
-        <v>1.5</v>
+        <v>1915.58</v>
       </c>
       <c r="E5" s="1">
-        <v>1915.58</v>
-      </c>
-      <c r="F5" s="1">
         <v>891</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2">
         <v>104.9</v>
       </c>
-      <c r="J5" s="3">
+      <c r="I5" s="3">
         <v>1864</v>
       </c>
-      <c r="K5" s="5">
+      <c r="J5" s="5">
         <v>7267</v>
       </c>
+      <c r="K5">
+        <v>169.99</v>
+      </c>
       <c r="L5">
-        <v>169.99</v>
+        <v>2.35</v>
       </c>
       <c r="M5">
-        <v>2.35</v>
+        <v>56.79</v>
       </c>
       <c r="N5">
-        <v>56.79</v>
+        <v>-0.9</v>
       </c>
       <c r="O5">
-        <v>-0.9</v>
+        <v>3.7702399999999998</v>
       </c>
       <c r="P5">
-        <v>3.7702399999999998</v>
+        <v>4.1839000000000004</v>
       </c>
       <c r="Q5">
-        <v>4.1839000000000004</v>
+        <v>302820517</v>
       </c>
       <c r="R5">
-        <v>302820517</v>
+        <v>620855</v>
       </c>
       <c r="S5">
-        <v>620855</v>
+        <v>7487761</v>
       </c>
       <c r="T5">
-        <v>7487761</v>
+        <v>20723423</v>
       </c>
       <c r="U5">
-        <v>20723423</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="V5">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="W5">
         <v>30.04</v>
       </c>
+      <c r="W5" s="6">
+        <v>66.83</v>
+      </c>
       <c r="X5" s="6">
-        <v>66.83</v>
+        <v>39.92</v>
       </c>
       <c r="Y5" s="6">
-        <v>39.92</v>
+        <v>11.95</v>
       </c>
       <c r="Z5" s="6">
-        <v>11.95</v>
+        <v>793.64</v>
       </c>
       <c r="AA5" s="6">
-        <v>793.64</v>
+        <v>1453.33</v>
       </c>
       <c r="AB5" s="6">
-        <v>1453.33</v>
+        <v>6.02</v>
       </c>
       <c r="AC5" s="6">
-        <v>6.02</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="AD5" s="6">
-        <v>1.1299999999999999</v>
+        <v>0.65</v>
       </c>
       <c r="AE5" s="6">
-        <v>0.65</v>
+        <v>21.54</v>
       </c>
       <c r="AF5" s="6">
-        <v>21.54</v>
-      </c>
-      <c r="AG5" s="6">
         <v>363.36</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2016</v>
       </c>
+      <c r="B6" s="1">
+        <v>222.225332044</v>
+      </c>
       <c r="C6" s="1">
-        <v>222.225332044</v>
+        <v>1.5</v>
       </c>
       <c r="D6" s="1">
-        <v>1.5</v>
+        <v>2017.18</v>
       </c>
       <c r="E6" s="1">
-        <v>2017.18</v>
-      </c>
-      <c r="F6" s="1">
         <v>1057</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1">
         <v>8550</v>
       </c>
-      <c r="I6" s="2">
+      <c r="H6" s="2">
         <v>106</v>
       </c>
-      <c r="J6" s="3">
+      <c r="I6" s="3">
         <v>1573</v>
       </c>
-      <c r="K6" s="5">
+      <c r="J6" s="5">
         <v>7422</v>
       </c>
+      <c r="K6">
+        <v>169.7</v>
+      </c>
       <c r="L6">
-        <v>169.7</v>
+        <v>3.74</v>
       </c>
       <c r="M6">
-        <v>3.74</v>
+        <v>60.09</v>
       </c>
       <c r="N6">
-        <v>60.09</v>
+        <v>-0.7</v>
       </c>
       <c r="O6">
-        <v>-0.7</v>
+        <v>3.9441099999999998</v>
       </c>
       <c r="P6">
-        <v>3.9441099999999998</v>
+        <v>4.3624999999999998</v>
       </c>
       <c r="Q6">
-        <v>4.3624999999999998</v>
+        <v>321977837</v>
       </c>
       <c r="R6">
-        <v>321977837</v>
+        <v>542843</v>
       </c>
       <c r="S6">
-        <v>542843</v>
+        <v>9331927</v>
       </c>
       <c r="T6">
-        <v>9331927</v>
+        <v>21675388</v>
       </c>
       <c r="U6">
-        <v>21675388</v>
+        <v>4.37</v>
       </c>
       <c r="V6">
-        <v>4.37</v>
-      </c>
-      <c r="W6">
         <v>28.02</v>
       </c>
+      <c r="W6" s="6">
+        <v>62.02</v>
+      </c>
       <c r="X6" s="6">
-        <v>62.02</v>
+        <v>38.409999999999997</v>
       </c>
       <c r="Y6" s="6">
-        <v>38.409999999999997</v>
+        <v>11.66</v>
       </c>
       <c r="Z6" s="6">
-        <v>11.66</v>
+        <v>905.5</v>
       </c>
       <c r="AA6" s="6">
-        <v>905.5</v>
+        <v>1851.83</v>
       </c>
       <c r="AB6" s="6">
-        <v>1851.83</v>
+        <v>5.91</v>
       </c>
       <c r="AC6" s="6">
-        <v>5.91</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="AD6" s="6">
-        <v>1.1100000000000001</v>
+        <v>0.62</v>
       </c>
       <c r="AE6" s="6">
-        <v>0.62</v>
+        <v>21.83</v>
       </c>
       <c r="AF6" s="6">
-        <v>21.83</v>
-      </c>
-      <c r="AG6" s="6">
         <v>355.15</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2017</v>
       </c>
+      <c r="B7" s="1">
+        <v>239.88541466064004</v>
+      </c>
       <c r="C7" s="1">
-        <v>239.88541466064004</v>
+        <v>1.5</v>
       </c>
       <c r="D7" s="1">
-        <v>1.5</v>
+        <v>2178.85</v>
       </c>
       <c r="E7" s="1">
-        <v>2178.85</v>
-      </c>
-      <c r="F7" s="1">
         <v>1289</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1">
         <v>9915</v>
       </c>
-      <c r="I7" s="2">
+      <c r="H7" s="2">
         <v>112.9</v>
       </c>
-      <c r="J7" s="3">
+      <c r="I7" s="3">
         <v>1819</v>
       </c>
-      <c r="K7" s="5">
+      <c r="J7" s="5">
         <v>7659</v>
       </c>
+      <c r="K7">
+        <v>163.69999999999999</v>
+      </c>
       <c r="L7">
-        <v>163.69999999999999</v>
+        <v>2.96</v>
       </c>
       <c r="M7">
-        <v>2.96</v>
+        <v>84.51</v>
       </c>
       <c r="N7">
-        <v>84.51</v>
+        <v>2.1</v>
       </c>
       <c r="O7">
-        <v>2.1</v>
+        <v>3.7793299999999999</v>
       </c>
       <c r="P7">
-        <v>3.7793299999999999</v>
+        <v>4.2576000000000001</v>
       </c>
       <c r="Q7">
-        <v>4.2576000000000001</v>
+        <v>347355323</v>
       </c>
       <c r="R7">
-        <v>347355323</v>
+        <v>438404</v>
       </c>
       <c r="S7">
-        <v>438404</v>
+        <v>9884497</v>
       </c>
       <c r="T7">
-        <v>9884497</v>
+        <v>22503579</v>
       </c>
       <c r="U7">
-        <v>22503579</v>
+        <v>4.63</v>
       </c>
       <c r="V7">
-        <v>4.63</v>
-      </c>
-      <c r="W7">
         <v>29.44</v>
       </c>
+      <c r="W7" s="6">
+        <v>66.44</v>
+      </c>
       <c r="X7" s="6">
-        <v>66.44</v>
+        <v>37.049999999999997</v>
       </c>
       <c r="Y7" s="6">
-        <v>37.049999999999997</v>
+        <v>9.56</v>
       </c>
       <c r="Z7" s="6">
-        <v>9.56</v>
+        <v>830.12</v>
       </c>
       <c r="AA7" s="6">
-        <v>830.12</v>
+        <v>1995.62</v>
       </c>
       <c r="AB7" s="6">
-        <v>1995.62</v>
+        <v>6.35</v>
       </c>
       <c r="AC7" s="6">
-        <v>6.35</v>
+        <v>1.39</v>
       </c>
       <c r="AD7" s="6">
-        <v>1.39</v>
+        <v>0.65</v>
       </c>
       <c r="AE7" s="6">
-        <v>0.65</v>
+        <v>21.64</v>
       </c>
       <c r="AF7" s="6">
-        <v>21.64</v>
-      </c>
-      <c r="AG7" s="6">
         <v>358.01</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2018</v>
       </c>
+      <c r="B8" s="1">
+        <v>250.25112177942833</v>
+      </c>
       <c r="C8" s="1">
-        <v>250.25112177942833</v>
+        <v>1.5</v>
       </c>
       <c r="D8" s="1">
-        <v>1.5</v>
+        <v>2290.29</v>
       </c>
       <c r="E8" s="1">
-        <v>2290.29</v>
-      </c>
-      <c r="F8" s="1">
         <v>1743</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1">
         <v>9230</v>
       </c>
-      <c r="I8" s="2">
+      <c r="H8" s="2">
         <v>110.9</v>
       </c>
-      <c r="J8" s="3">
+      <c r="I8" s="3">
         <v>2219.5</v>
       </c>
-      <c r="K8" s="5">
+      <c r="J8" s="5">
         <v>7824</v>
       </c>
+      <c r="K8">
+        <v>194.3</v>
+      </c>
       <c r="L8">
-        <v>194.3</v>
+        <v>2.96</v>
       </c>
       <c r="M8">
-        <v>2.96</v>
+        <v>91.83</v>
       </c>
       <c r="N8">
-        <v>91.83</v>
+        <v>1.8</v>
       </c>
       <c r="O8">
-        <v>1.8</v>
+        <v>3.6114000000000002</v>
       </c>
       <c r="P8">
-        <v>3.6114000000000002</v>
+        <v>4.2622999999999998</v>
       </c>
       <c r="Q8">
-        <v>4.2622999999999998</v>
+        <v>378305207</v>
       </c>
       <c r="R8">
-        <v>378305207</v>
+        <v>383301</v>
       </c>
       <c r="S8">
-        <v>383301</v>
+        <v>10017749</v>
       </c>
       <c r="T8">
-        <v>10017749</v>
+        <v>23429016</v>
       </c>
       <c r="U8">
-        <v>23429016</v>
+        <v>4.95</v>
       </c>
       <c r="V8">
-        <v>4.95</v>
-      </c>
-      <c r="W8">
         <v>30.14</v>
       </c>
+      <c r="W8" s="6">
+        <v>72.62</v>
+      </c>
       <c r="X8" s="6">
-        <v>72.62</v>
+        <v>42.58</v>
       </c>
       <c r="Y8" s="6">
-        <v>42.58</v>
+        <v>10.53</v>
       </c>
       <c r="Z8" s="6">
-        <v>10.53</v>
+        <v>956.84</v>
       </c>
       <c r="AA8" s="6">
-        <v>956.84</v>
+        <v>1970.59</v>
       </c>
       <c r="AB8" s="6">
-        <v>1970.59</v>
+        <v>6.58</v>
       </c>
       <c r="AC8" s="6">
-        <v>6.58</v>
+        <v>1.35</v>
       </c>
       <c r="AD8" s="6">
-        <v>1.35</v>
+        <v>0.65</v>
       </c>
       <c r="AE8" s="6">
-        <v>0.65</v>
+        <v>21.97</v>
       </c>
       <c r="AF8" s="6">
-        <v>21.97</v>
-      </c>
-      <c r="AG8" s="6">
         <v>389.86</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2019</v>
       </c>
+      <c r="B9" s="1">
+        <v>236.3962704762196</v>
+      </c>
       <c r="C9" s="1">
-        <v>236.3962704762196</v>
+        <v>1.5</v>
       </c>
       <c r="D9" s="1">
-        <v>1.5</v>
+        <v>2373.16</v>
       </c>
       <c r="E9" s="1">
-        <v>2373.16</v>
-      </c>
-      <c r="F9" s="1">
         <v>789</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1">
         <v>8625</v>
       </c>
-      <c r="I9" s="2">
+      <c r="H9" s="2">
         <v>106.6</v>
       </c>
-      <c r="J9" s="3">
+      <c r="I9" s="3">
         <v>1910</v>
       </c>
-      <c r="K9" s="5">
+      <c r="J9" s="5">
         <v>8247</v>
       </c>
+      <c r="K9">
+        <v>245.44</v>
+      </c>
       <c r="L9">
-        <v>245.44</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="M9">
-        <v>2.1800000000000002</v>
+        <v>60.17</v>
       </c>
       <c r="N9">
-        <v>60.17</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="O9">
-        <v>2.2000000000000002</v>
+        <v>3.83948</v>
       </c>
       <c r="P9">
-        <v>3.83948</v>
+        <v>4.298</v>
       </c>
       <c r="Q9">
-        <v>4.298</v>
+        <v>409628944</v>
       </c>
       <c r="R9">
-        <v>409628944</v>
+        <v>328880</v>
       </c>
       <c r="S9">
-        <v>328880</v>
+        <v>10317711</v>
       </c>
       <c r="T9">
-        <v>10317711</v>
+        <v>24360166</v>
       </c>
       <c r="U9">
-        <v>24360166</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="V9">
-        <v>5.0199999999999996</v>
-      </c>
-      <c r="W9">
         <v>31.81</v>
       </c>
+      <c r="W9" s="6">
+        <v>72.260000000000005</v>
+      </c>
       <c r="X9" s="6">
-        <v>72.260000000000005</v>
+        <v>58.33</v>
       </c>
       <c r="Y9" s="6">
-        <v>58.33</v>
+        <v>10.67</v>
       </c>
       <c r="Z9" s="6">
-        <v>10.67</v>
+        <v>1016.64</v>
       </c>
       <c r="AA9" s="6">
-        <v>1016.64</v>
+        <v>1891.62</v>
       </c>
       <c r="AB9" s="6">
-        <v>1891.62</v>
+        <v>6.33</v>
       </c>
       <c r="AC9" s="6">
-        <v>6.33</v>
+        <v>1.35</v>
       </c>
       <c r="AD9" s="6">
-        <v>1.35</v>
+        <v>0.6</v>
       </c>
       <c r="AE9" s="6">
-        <v>0.6</v>
+        <v>22.43</v>
       </c>
       <c r="AF9" s="6">
-        <v>22.43</v>
-      </c>
-      <c r="AG9" s="6">
         <v>397.24</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2020</v>
       </c>
+      <c r="B10" s="1">
+        <v>223.24188901277105</v>
+      </c>
       <c r="C10" s="1">
-        <v>223.24188901277105</v>
+        <v>0.1</v>
       </c>
       <c r="D10" s="1">
-        <v>0.1</v>
+        <v>2522.38</v>
       </c>
       <c r="E10" s="1">
-        <v>2522.38</v>
-      </c>
-      <c r="F10" s="1">
         <v>715</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1">
         <v>6400</v>
       </c>
-      <c r="I10" s="2">
+      <c r="H10" s="2">
         <v>99.1</v>
       </c>
-      <c r="J10" s="3">
+      <c r="I10" s="3">
         <v>1722</v>
       </c>
-      <c r="K10" s="5">
+      <c r="J10" s="5">
         <v>9228</v>
       </c>
+      <c r="K10">
+        <v>252.69</v>
+      </c>
       <c r="L10">
-        <v>252.69</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="M10">
-        <v>2.4300000000000002</v>
+        <v>50.13</v>
       </c>
       <c r="N10">
-        <v>50.13</v>
+        <v>3.4</v>
       </c>
       <c r="O10">
-        <v>3.4</v>
+        <v>3.8994499999999999</v>
       </c>
       <c r="P10">
-        <v>3.8994499999999999</v>
+        <v>4.4447999999999999</v>
       </c>
       <c r="Q10">
-        <v>4.4447999999999999</v>
+        <v>422809674</v>
       </c>
       <c r="R10">
-        <v>422809674</v>
+        <v>415520</v>
       </c>
       <c r="S10">
-        <v>415520</v>
+        <v>10795848</v>
       </c>
       <c r="T10">
-        <v>10795848</v>
+        <v>25113862</v>
       </c>
       <c r="U10">
-        <v>25113862</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="V10">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="W10">
         <v>33.61</v>
       </c>
+      <c r="W10" s="6">
+        <v>74.86</v>
+      </c>
       <c r="X10" s="6">
-        <v>74.86</v>
+        <v>44.82</v>
       </c>
       <c r="Y10" s="6">
-        <v>44.82</v>
+        <v>10.19</v>
       </c>
       <c r="Z10" s="6">
-        <v>10.19</v>
+        <v>1035.99</v>
       </c>
       <c r="AA10" s="6">
-        <v>1035.99</v>
+        <v>1663.87</v>
       </c>
       <c r="AB10" s="6">
-        <v>1663.87</v>
+        <v>6.4</v>
       </c>
       <c r="AC10" s="6">
-        <v>6.4</v>
+        <v>1.38</v>
       </c>
       <c r="AD10" s="6">
-        <v>1.38</v>
+        <v>0.67</v>
       </c>
       <c r="AE10" s="6">
-        <v>0.67</v>
+        <v>23.38</v>
       </c>
       <c r="AF10" s="6">
-        <v>23.38</v>
-      </c>
-      <c r="AG10" s="6">
         <v>402.43</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2021</v>
       </c>
+      <c r="B11" s="1">
+        <v>243.63311201119035</v>
+      </c>
       <c r="C11" s="1">
-        <v>243.63311201119035</v>
+        <v>1.75</v>
       </c>
       <c r="D11" s="1">
-        <v>1.75</v>
+        <v>2805.81</v>
       </c>
       <c r="E11" s="1">
-        <v>2805.81</v>
-      </c>
-      <c r="F11" s="1">
         <v>954</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1">
         <v>7955</v>
       </c>
-      <c r="I11" s="2">
+      <c r="H11" s="2">
         <v>122.5</v>
       </c>
-      <c r="J11" s="1">
+      <c r="I11" s="1">
         <v>1977.5</v>
       </c>
-      <c r="K11" s="6">
+      <c r="J11" s="6">
         <v>10073.09</v>
       </c>
+      <c r="K11">
+        <v>278.08</v>
+      </c>
       <c r="L11">
-        <v>278.08</v>
+        <v>3.76</v>
       </c>
       <c r="M11">
-        <v>3.76</v>
+        <v>122.6</v>
       </c>
       <c r="N11">
-        <v>122.6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="O11">
-        <v>5.0999999999999996</v>
+        <v>3.8608699999999998</v>
       </c>
       <c r="P11">
-        <v>3.8608699999999998</v>
+        <v>4.5674000000000001</v>
       </c>
       <c r="Q11">
-        <v>4.5674000000000001</v>
+        <v>470293984</v>
       </c>
       <c r="R11">
-        <v>470293984</v>
+        <v>427531</v>
       </c>
       <c r="S11">
-        <v>427531</v>
+        <v>11009520</v>
       </c>
       <c r="T11">
-        <v>11009520</v>
+        <v>25869804</v>
       </c>
       <c r="U11">
-        <v>25869804</v>
+        <v>5.49</v>
       </c>
       <c r="V11">
-        <v>5.49</v>
-      </c>
-      <c r="W11">
         <v>33.520000000000003</v>
       </c>
+      <c r="W11" s="6">
+        <v>96.76</v>
+      </c>
       <c r="X11" s="6">
-        <v>96.76</v>
+        <v>45.51</v>
       </c>
       <c r="Y11" s="6">
-        <v>45.51</v>
+        <v>12.24</v>
       </c>
       <c r="Z11" s="6">
-        <v>12.24</v>
+        <v>1168.8</v>
       </c>
       <c r="AA11" s="6">
-        <v>1168.8</v>
+        <v>1552.84</v>
       </c>
       <c r="AB11" s="6">
-        <v>1552.84</v>
+        <v>7.63</v>
       </c>
       <c r="AC11" s="6">
-        <v>7.63</v>
+        <v>1.57</v>
       </c>
       <c r="AD11" s="6">
-        <v>1.57</v>
+        <v>0.74</v>
       </c>
       <c r="AE11" s="6">
-        <v>0.74</v>
+        <v>24.28</v>
       </c>
       <c r="AF11" s="6">
-        <v>24.28</v>
-      </c>
-      <c r="AG11" s="6">
         <v>415.26</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2022</v>
       </c>
       <c r="B12" s="1">
-        <v>1618559.3</v>
+        <v>248.5420552846804</v>
       </c>
       <c r="C12" s="1">
-        <v>248.5420552846804</v>
+        <v>6.75</v>
       </c>
       <c r="D12" s="1">
-        <v>6.75</v>
+        <v>3110.03</v>
       </c>
       <c r="E12" s="1">
-        <v>3110.03</v>
-      </c>
-      <c r="F12" s="1">
         <v>841</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1">
         <v>8765</v>
       </c>
-      <c r="I12" s="2">
+      <c r="H12" s="2">
         <v>135.9</v>
       </c>
-      <c r="J12" s="3">
+      <c r="I12" s="3">
         <v>3021</v>
       </c>
-      <c r="K12" s="5">
+      <c r="J12" s="5">
         <v>11382</v>
       </c>
+      <c r="K12">
+        <v>523.71</v>
+      </c>
       <c r="L12">
-        <v>523.71</v>
+        <v>4.08</v>
       </c>
       <c r="M12">
-        <v>4.08</v>
+        <v>291.27999999999997</v>
       </c>
       <c r="N12">
-        <v>291.27999999999997</v>
+        <v>14.4</v>
       </c>
       <c r="O12">
-        <v>14.4</v>
+        <v>4.4577499999999999</v>
       </c>
       <c r="P12">
-        <v>4.4577499999999999</v>
+        <v>4.6868999999999996</v>
       </c>
       <c r="Q12">
-        <v>4.6868999999999996</v>
+        <v>538020334</v>
       </c>
       <c r="R12">
-        <v>538020334</v>
+        <v>328664</v>
       </c>
       <c r="S12">
-        <v>328664</v>
+        <v>11397576</v>
       </c>
       <c r="T12">
-        <v>11397576</v>
+        <v>26457659</v>
       </c>
       <c r="U12">
-        <v>26457659</v>
+        <v>6.67</v>
       </c>
       <c r="V12">
-        <v>6.67</v>
-      </c>
-      <c r="W12">
         <v>26.63</v>
       </c>
+      <c r="W12" s="6">
+        <v>151.99</v>
+      </c>
       <c r="X12" s="6">
-        <v>151.99</v>
+        <v>69.849999999999994</v>
       </c>
       <c r="Y12" s="6">
-        <v>69.849999999999994</v>
+        <v>19.5</v>
       </c>
       <c r="Z12" s="6">
-        <v>19.5</v>
+        <v>1768.83</v>
       </c>
       <c r="AA12" s="6">
-        <v>1768.83</v>
+        <v>1724.31</v>
       </c>
       <c r="AB12" s="6">
-        <v>1724.31</v>
+        <v>10.48</v>
       </c>
       <c r="AC12" s="6">
-        <v>10.48</v>
+        <v>2.31</v>
       </c>
       <c r="AD12" s="6">
-        <v>2.31</v>
+        <v>0.77</v>
       </c>
       <c r="AE12" s="6">
-        <v>0.77</v>
+        <v>28.81</v>
       </c>
       <c r="AF12" s="6">
-        <v>28.81</v>
-      </c>
-      <c r="AG12" s="6">
         <v>470.51</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
       <c r="B13" s="1">
-        <v>1613393.1</v>
+        <v>231.6088983613767</v>
       </c>
       <c r="C13" s="1">
-        <v>231.6088983613767</v>
+        <v>5.75</v>
       </c>
       <c r="D13" s="1">
-        <v>5.75</v>
+        <v>3162.01</v>
       </c>
       <c r="E13" s="1">
-        <v>3162.01</v>
-      </c>
-      <c r="F13" s="1">
         <v>641</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="1">
         <v>8353</v>
       </c>
-      <c r="I13" s="2">
+      <c r="H13" s="2">
         <v>81.900000000000006</v>
       </c>
-      <c r="J13" s="1">
+      <c r="I13" s="1">
         <v>2644</v>
       </c>
-      <c r="K13" s="5">
+      <c r="J13" s="5">
         <v>11704</v>
       </c>
+      <c r="K13">
+        <v>759.29</v>
+      </c>
       <c r="L13">
-        <v>759.29</v>
+        <v>2.5</v>
       </c>
       <c r="M13">
-        <v>2.5</v>
+        <v>129.54</v>
       </c>
       <c r="N13">
-        <v>129.54</v>
+        <v>11.5</v>
       </c>
       <c r="O13">
-        <v>11.5</v>
+        <v>4.2016900000000001</v>
       </c>
       <c r="P13">
-        <v>4.2016900000000001</v>
+        <v>4.5430000000000001</v>
       </c>
       <c r="Q13">
-        <v>4.5430000000000001</v>
+        <v>604247135</v>
       </c>
       <c r="R13">
-        <v>604247135</v>
+        <v>299738</v>
       </c>
       <c r="S13">
-        <v>299738</v>
+        <v>12329365</v>
       </c>
       <c r="T13">
-        <v>12329365</v>
+        <v>27227691</v>
       </c>
       <c r="U13">
-        <v>27227691</v>
+        <v>6.58</v>
       </c>
       <c r="V13">
-        <v>6.58</v>
-      </c>
-      <c r="W13">
         <v>36.64</v>
       </c>
+      <c r="W13" s="6">
+        <v>98.79</v>
+      </c>
       <c r="X13" s="6">
-        <v>98.79</v>
+        <v>91.37</v>
       </c>
       <c r="Y13" s="6">
-        <v>91.37</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="Z13" s="6">
-        <v>18.989999999999998</v>
+        <v>2244.8000000000002</v>
       </c>
       <c r="AA13" s="6">
-        <v>2244.8000000000002</v>
+        <v>2149.96</v>
       </c>
       <c r="AB13" s="6">
-        <v>2149.96</v>
+        <v>10.39</v>
       </c>
       <c r="AC13" s="6">
-        <v>10.39</v>
+        <v>2.08</v>
       </c>
       <c r="AD13" s="6">
-        <v>2.08</v>
+        <v>0.91</v>
       </c>
       <c r="AE13" s="6">
-        <v>0.91</v>
+        <v>39.520000000000003</v>
       </c>
       <c r="AF13" s="6">
-        <v>39.520000000000003</v>
-      </c>
-      <c r="AG13" s="6">
         <v>518.1</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2024</v>
       </c>
       <c r="B14" s="1">
-        <v>1523353.8</v>
+        <v>223.56184830002925</v>
       </c>
       <c r="C14" s="1">
-        <v>223.56184830002925</v>
+        <v>5.75</v>
       </c>
       <c r="D14" s="1">
-        <v>5.75</v>
+        <v>3504.24</v>
       </c>
       <c r="E14" s="1">
-        <v>3504.24</v>
-      </c>
-      <c r="F14" s="1">
         <v>826</v>
       </c>
-      <c r="H14" s="1">
+      <c r="G14" s="1">
         <v>8088</v>
       </c>
-      <c r="I14" s="2">
+      <c r="H14" s="2">
         <v>99.8</v>
       </c>
-      <c r="J14" s="1">
+      <c r="I14" s="1">
         <v>2280</v>
       </c>
-      <c r="K14" s="5">
+      <c r="J14" s="5">
         <v>13986</v>
       </c>
+      <c r="K14">
+        <v>518.80999999999995</v>
+      </c>
       <c r="L14">
-        <v>518.80999999999995</v>
+        <v>3.64</v>
       </c>
       <c r="M14">
-        <v>3.64</v>
+        <v>112</v>
       </c>
       <c r="N14">
-        <v>112</v>
+        <v>3.8</v>
       </c>
       <c r="O14">
-        <v>3.8</v>
+        <v>3.9813299999999998</v>
       </c>
       <c r="P14">
-        <v>3.9813299999999998</v>
+        <v>4.3064</v>
       </c>
       <c r="Q14">
-        <v>4.3064</v>
+        <v>678626024</v>
       </c>
       <c r="R14">
-        <v>678626024</v>
+        <v>298052</v>
       </c>
       <c r="S14">
-        <v>298052</v>
+        <v>14718155</v>
       </c>
       <c r="T14">
-        <v>14718155</v>
+        <v>22951213</v>
       </c>
       <c r="U14">
-        <v>22951213</v>
+        <v>6.44</v>
       </c>
       <c r="V14">
-        <v>6.44</v>
-      </c>
-      <c r="W14">
         <v>35.71</v>
       </c>
+      <c r="W14" s="6">
+        <v>82.62</v>
+      </c>
       <c r="X14" s="6">
-        <v>82.62</v>
+        <v>86.84</v>
       </c>
       <c r="Y14" s="6">
-        <v>86.84</v>
+        <v>17.64</v>
       </c>
       <c r="Z14" s="6">
-        <v>17.64</v>
+        <v>1873.75</v>
       </c>
       <c r="AA14" s="6">
-        <v>1873.75</v>
+        <v>1792.26</v>
       </c>
       <c r="AB14" s="6">
-        <v>1792.26</v>
+        <v>10.62</v>
       </c>
       <c r="AC14" s="6">
-        <v>10.62</v>
+        <v>2.11</v>
       </c>
       <c r="AD14" s="6">
-        <v>2.11</v>
+        <v>1.01</v>
       </c>
       <c r="AE14" s="6">
-        <v>1.01</v>
+        <v>41.83</v>
       </c>
       <c r="AF14" s="6">
-        <v>41.83</v>
-      </c>
-      <c r="AG14" s="6">
         <v>545.16</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C15" s="1">
-        <v>180.95164108254602</v>
-      </c>
-      <c r="D15" s="1">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3724.13</v>
-      </c>
-      <c r="F15" s="1">
-        <v>904</v>
-      </c>
-      <c r="H15" s="1">
-        <v>7069</v>
-      </c>
-      <c r="J15" s="3">
-        <v>2595.3000000000002</v>
-      </c>
-      <c r="K15" s="5">
-        <v>14791</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="M15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N15" t="s">
-        <v>46</v>
-      </c>
-      <c r="O15" t="s">
-        <v>47</v>
-      </c>
-      <c r="P15" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>49</v>
-      </c>
-      <c r="R15" t="s">
-        <v>50</v>
-      </c>
-      <c r="S15" t="s">
-        <v>50</v>
-      </c>
-      <c r="T15" t="s">
-        <v>50</v>
-      </c>
-      <c r="U15" t="s">
-        <v>50</v>
-      </c>
-      <c r="V15" t="s">
-        <v>50</v>
-      </c>
-      <c r="W15" t="s">
-        <v>51</v>
-      </c>
-      <c r="X15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>50</v>
-      </c>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="I15" s="3"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="7"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
     </row>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="133" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="134" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="140" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="141" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="142" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="149" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="150" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="151" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="152" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="153" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="154" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="155" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="156" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="157" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="158" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="159" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="160" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="161" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="162" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="163" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="164" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="165" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="166" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="167" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="168" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="169" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="170" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="171" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="172" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="173" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="174" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A5">
     <sortCondition ref="A3:A5"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56504921-3E6C-414B-8F65-4C1804DBE78B}">
+  <dimension ref="A4:AF4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="1">
+        <v>180.95164108254602</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3724.13</v>
+      </c>
+      <c r="E4" s="1">
+        <v>904</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7069</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2595.3000000000002</v>
+      </c>
+      <c r="J4" s="5">
+        <v>14791</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" t="s">
+        <v>49</v>
+      </c>
+      <c r="U4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4" t="s">
+        <v>50</v>
+      </c>
+      <c r="W4" t="s">
+        <v>49</v>
+      </c>
+      <c r="X4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <hyperlinks>
-    <hyperlink ref="L15" r:id="rId1" xr:uid="{82CD74E8-47B6-4E5E-834D-3D0267E39A03}"/>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{E75F7872-3DE4-DF4B-9B00-2F21FCAB44AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
polynomial fixed and forecast added
</commit_message>
<xml_diff>
--- a/data/DATA_PKD_SPECIFIC.xlsx
+++ b/data/DATA_PKD_SPECIFIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Documents/competitions/hackatons/hacknation_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C2F80D-31BA-5340-A339-E3D6F26277F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF7B880-02B3-514E-98B4-FFA5E5DFEBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -254,7 +254,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -267,6 +267,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperłącze" xfId="2" builtinId="8"/>
@@ -552,7 +553,7 @@
   <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -681,6 +682,9 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G2" s="1">
+        <v>7732</v>
+      </c>
       <c r="H2" s="2">
         <v>103</v>
       </c>
@@ -776,6 +780,9 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G3" s="1">
+        <v>8014</v>
+      </c>
       <c r="H3" s="2">
         <v>103.5</v>
       </c>
@@ -871,6 +878,9 @@
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G4" s="1">
+        <v>7436</v>
+      </c>
       <c r="H4" s="2">
         <v>100.7</v>
       </c>
@@ -966,6 +976,9 @@
       <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="G5" s="1">
+        <v>8312</v>
+      </c>
       <c r="H5" s="2">
         <v>104.9</v>
       </c>
@@ -1841,6 +1854,9 @@
       </c>
       <c r="E14" s="1">
         <v>826</v>
+      </c>
+      <c r="F14" s="8">
+        <v>13671.43</v>
       </c>
       <c r="G14" s="1">
         <v>8088</v>

</xml_diff>